<commit_message>
Onkologia & Anestezjologia source file corrected
</commit_message>
<xml_diff>
--- a/txt_to_json_converter/Rozpiska tygodni.xlsx
+++ b/txt_to_json_converter/Rozpiska tygodni.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studia\projekty\UMlub-nie-umie-w-plan-lekcji\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studia\projekty\UMlub-nie-umie-w-plan-lekcji\txt_to_json_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E074350A-755B-4354-BE2A-4DD7A0D52056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABDF76C-2D9C-4C73-ABBC-907CB15752D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{12D9AF85-2611-4F3D-942B-AD4D16DF0EAB}"/>
   </bookViews>
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -143,6 +143,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -480,7 +483,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="L6" activeCellId="2" sqref="A6:F6 K7:N7 L6"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1026,7 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="12">
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
@@ -1096,7 +1099,7 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>

</xml_diff>